<commit_message>
Added : SignUp test (with cross browser checking)
</commit_message>
<xml_diff>
--- a/KeywordDrivenTest/src/main/java/com/keyworddriven/scenario/Fb_scenarios.xlsx
+++ b/KeywordDrivenTest/src/main/java/com/keyworddriven/scenario/Fb_scenarios.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwetamahajan\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E746103-12BE-4EB1-AF1C-47B5CDEDBE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A9B5F7-15DC-485F-8AF9-DE068F45B8AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4FFD32F5-DC3C-4B58-853D-2B352DF04357}"/>
   </bookViews>
   <sheets>
     <sheet name="FbLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="SignUp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>teststep</t>
   </si>
@@ -62,9 +63,6 @@
     <t>enter url</t>
   </si>
   <si>
-    <t>https://www.facebook.com/</t>
-  </si>
-  <si>
     <t>enter email</t>
   </si>
   <si>
@@ -99,13 +97,31 @@
   </si>
   <si>
     <t>quit</t>
+  </si>
+  <si>
+    <t>verify login page</t>
+  </si>
+  <si>
+    <t>get title</t>
+  </si>
+  <si>
+    <t>verify sign up link</t>
+  </si>
+  <si>
+    <t>linkText=Sign Up</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,18 +149,25 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,11 +187,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -185,14 +209,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B8A8A652-8B6C-4B5F-BA0A-7B944C707ED8}"/>
   </cellStyles>
@@ -506,18 +535,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E059BD0B-3122-4DAE-90FD-011B98B5B663}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -546,7 +575,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -559,47 +588,47 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
+      <c r="D3" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -607,15 +636,29 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -623,6 +666,100 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80119AF-5EBA-48FA-92AD-A6965B364AF1}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="4" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{B6AAC7F4-B886-4B83-84E7-19821B7AFF4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>